<commit_message>
Fri Jan 31 17:26:38 CET 2025
</commit_message>
<xml_diff>
--- a/_GPO/Progetto/Verde/Gantt 5IB - VERDE.xlsx
+++ b/_GPO/Progetto/Verde/Gantt 5IB - VERDE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28521"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://istitutogreppi-my.sharepoint.com/personal/margherita_sironi_issgreppi_it/Documents/Documenti/Marghe/gpo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/origgi/Desktop/StefanoOriggi/_GPO/Progetto/Verde/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="8_{6CA74AD4-84F1-4D54-8AD4-D8EEC76DF9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFC61365-206D-4AB6-82EF-6AAC9B9730F9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573A6A35-30DE-6F4D-8946-7BCB07718393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="32360" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart Template" sheetId="1" r:id="rId1"/>
@@ -166,7 +166,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -312,31 +312,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF76A5AF"/>
-          <bgColor rgb="FF76A5AF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -678,56 +662,56 @@
   </sheetPr>
   <dimension ref="A1:DA24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="53" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="159" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="131" width="4.5703125" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="131" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:105" ht="91.5" customHeight="1">
+    <row r="1" spans="1:105" ht="91.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="17"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="19"/>
-      <c r="AH1" s="19"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
+      <c r="AG1" s="18"/>
+      <c r="AH1" s="18"/>
       <c r="AI1" s="4"/>
       <c r="AJ1" s="4"/>
       <c r="AK1" s="4"/>
@@ -767,7 +751,7 @@
       <c r="BS1" s="4"/>
       <c r="BT1" s="4"/>
     </row>
-    <row r="2" spans="1:105" ht="66">
+    <row r="2" spans="1:105" ht="63" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -1082,7 +1066,7 @@
         <v>45782</v>
       </c>
     </row>
-    <row r="3" spans="1:105" ht="13.5">
+    <row r="3" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="8" t="s">
         <v>5</v>
@@ -1199,7 +1183,7 @@
       <c r="CZ3" s="11"/>
       <c r="DA3" s="13"/>
     </row>
-    <row r="4" spans="1:105" ht="13.5">
+    <row r="4" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="15" t="s">
         <v>8</v>
@@ -1316,7 +1300,7 @@
       <c r="CZ4" s="11"/>
       <c r="DA4" s="13"/>
     </row>
-    <row r="5" spans="1:105" ht="13.5">
+    <row r="5" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="15" t="s">
         <v>11</v>
@@ -1433,7 +1417,7 @@
       <c r="CZ5" s="11"/>
       <c r="DA5" s="13"/>
     </row>
-    <row r="6" spans="1:105" ht="13.5">
+    <row r="6" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="15" t="s">
         <v>13</v>
@@ -1550,7 +1534,7 @@
       <c r="CZ6" s="11"/>
       <c r="DA6" s="13"/>
     </row>
-    <row r="7" spans="1:105" ht="13.5">
+    <row r="7" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="15" t="s">
         <v>16</v>
@@ -1667,7 +1651,7 @@
       <c r="CZ7" s="11"/>
       <c r="DA7" s="13"/>
     </row>
-    <row r="8" spans="1:105" ht="13.5">
+    <row r="8" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="15" t="s">
         <v>18</v>
@@ -1784,7 +1768,7 @@
       <c r="CZ8" s="11"/>
       <c r="DA8" s="13"/>
     </row>
-    <row r="9" spans="1:105" ht="13.5">
+    <row r="9" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="15" t="s">
         <v>20</v>
@@ -1901,7 +1885,7 @@
       <c r="CZ9" s="11"/>
       <c r="DA9" s="13"/>
     </row>
-    <row r="10" spans="1:105" ht="13.5">
+    <row r="10" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="15" t="s">
         <v>22</v>
@@ -2018,7 +2002,7 @@
       <c r="CZ10" s="11"/>
       <c r="DA10" s="13"/>
     </row>
-    <row r="11" spans="1:105" ht="13.5">
+    <row r="11" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="15" t="s">
         <v>24</v>
@@ -2135,7 +2119,7 @@
       <c r="CZ11" s="11"/>
       <c r="DA11" s="13"/>
     </row>
-    <row r="12" spans="1:105" ht="13.5">
+    <row r="12" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="15" t="s">
         <v>25</v>
@@ -2252,7 +2236,7 @@
       <c r="CZ12" s="11"/>
       <c r="DA12" s="13"/>
     </row>
-    <row r="13" spans="1:105" ht="13.5">
+    <row r="13" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="15" t="s">
         <v>27</v>
@@ -2369,7 +2353,7 @@
       <c r="CZ13" s="11"/>
       <c r="DA13" s="13"/>
     </row>
-    <row r="14" spans="1:105" ht="13.5">
+    <row r="14" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="15" t="s">
         <v>28</v>
@@ -2486,7 +2470,7 @@
       <c r="CZ14" s="11"/>
       <c r="DA14" s="13"/>
     </row>
-    <row r="15" spans="1:105" ht="13.5">
+    <row r="15" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="15" t="s">
         <v>29</v>
@@ -2603,7 +2587,7 @@
       <c r="CZ15" s="11"/>
       <c r="DA15" s="13"/>
     </row>
-    <row r="16" spans="1:105" ht="13.5">
+    <row r="16" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="15" t="s">
         <v>30</v>
@@ -2720,7 +2704,7 @@
       <c r="CZ16" s="11"/>
       <c r="DA16" s="13"/>
     </row>
-    <row r="17" spans="1:105" ht="13.5">
+    <row r="17" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="15" t="s">
         <v>31</v>
@@ -2837,7 +2821,7 @@
       <c r="CZ17" s="11"/>
       <c r="DA17" s="13"/>
     </row>
-    <row r="18" spans="1:105" ht="13.5">
+    <row r="18" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="15" t="s">
         <v>32</v>
@@ -2954,7 +2938,7 @@
       <c r="CZ18" s="11"/>
       <c r="DA18" s="13"/>
     </row>
-    <row r="19" spans="1:105" ht="13.5">
+    <row r="19" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="15" t="s">
         <v>33</v>
@@ -3071,7 +3055,7 @@
       <c r="CZ19" s="11"/>
       <c r="DA19" s="13"/>
     </row>
-    <row r="20" spans="1:105" ht="13.5">
+    <row r="20" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="15" t="s">
         <v>34</v>
@@ -3188,7 +3172,7 @@
       <c r="CZ20" s="11"/>
       <c r="DA20" s="13"/>
     </row>
-    <row r="21" spans="1:105" ht="13.5">
+    <row r="21" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="15" t="s">
         <v>35</v>
@@ -3305,7 +3289,7 @@
       <c r="CZ21" s="11"/>
       <c r="DA21" s="13"/>
     </row>
-    <row r="22" spans="1:105" ht="13.5">
+    <row r="22" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="15" t="s">
         <v>36</v>
@@ -3422,7 +3406,7 @@
       <c r="CZ22" s="11"/>
       <c r="DA22" s="13"/>
     </row>
-    <row r="23" spans="1:105" ht="13.5">
+    <row r="23" spans="1:105" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="15" t="s">
         <v>37</v>
@@ -3539,7 +3523,7 @@
       <c r="CZ23" s="11"/>
       <c r="DA23" s="13"/>
     </row>
-    <row r="24" spans="1:105" ht="15.75" customHeight="1">
+    <row r="24" spans="1:105" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="15" t="s">
         <v>38</v>
       </c>
@@ -3661,20 +3645,12 @@
     <mergeCell ref="L1:AH1"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="G3:DA23">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="3">
+  <conditionalFormatting sqref="G3:DA24">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(G3))&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>AND($C3&lt;=G$2,$D3&gt;=G$2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G24:DA24">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(G24))&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AND($C24&lt;=G$2,$D24&gt;=G$2)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -3722,13 +3698,13 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>39</v>
       </c>
@@ -3736,7 +3712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
@@ -3744,7 +3720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>26</v>
       </c>
@@ -3752,7 +3728,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>14</v>
       </c>
@@ -3760,7 +3736,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>17</v>
       </c>
@@ -3768,7 +3744,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
         <v>19</v>
       </c>
@@ -3776,7 +3752,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
         <v>21</v>
       </c>
@@ -3784,7 +3760,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
         <v>23</v>
       </c>
@@ -3803,26 +3779,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b98c3651-2320-4920-a81d-baad65de77d3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cb577c89-241a-4dd6-8c77-1faea3b86602">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C240D8F7A7575D4BACE6D8DC8CE2699D" ma:contentTypeVersion="11" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7bd0d3821f30cec562649af6727d5044">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cb577c89-241a-4dd6-8c77-1faea3b86602" xmlns:ns3="b98c3651-2320-4920-a81d-baad65de77d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ce9dba49ee2a04c2b3827884fb94a204" ns2:_="" ns3:_="">
     <xsd:import namespace="cb577c89-241a-4dd6-8c77-1faea3b86602"/>
@@ -4017,14 +3973,60 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b98c3651-2320-4920-a81d-baad65de77d3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cb577c89-241a-4dd6-8c77-1faea3b86602">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{943F14EF-0DE2-4C9B-9B95-0243A8BE8F47}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79AFCA36-FA8F-4341-8145-41632AC30DA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cb577c89-241a-4dd6-8c77-1faea3b86602"/>
+    <ds:schemaRef ds:uri="b98c3651-2320-4920-a81d-baad65de77d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{267A8F49-73B7-40B7-A71D-FBF562DC685D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{267A8F49-73B7-40B7-A71D-FBF562DC685D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79AFCA36-FA8F-4341-8145-41632AC30DA7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{943F14EF-0DE2-4C9B-9B95-0243A8BE8F47}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b98c3651-2320-4920-a81d-baad65de77d3"/>
+    <ds:schemaRef ds:uri="cb577c89-241a-4dd6-8c77-1faea3b86602"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>